<commit_message>
Implemented run script buttons
</commit_message>
<xml_diff>
--- a/scraplingAdaptationHana/giant/giant_price_compare/giant_foods_comparison.xlsx
+++ b/scraplingAdaptationHana/giant/giant_price_compare/giant_foods_comparison.xlsx
@@ -478,631 +478,631 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>16000124790</v>
+        <v>20735092767</v>
       </c>
       <c r="B2" t="n">
-        <v>6.99</v>
+        <v>2.79</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1600012479</t>
+          <t>2073509276</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1600012479</v>
+        <v>2073509276</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>2.29</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Cheerios Gluten Free Honey Nut Cereal</t>
+          <t>Turkey Hill Lemonade</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-06-10T14:13:19.085881</t>
+          <t>2025-06-10T13:40:05.953709</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>20735092767</v>
+        <v>14800000344</v>
       </c>
       <c r="B3" t="n">
-        <v>2.79</v>
+        <v>4.99</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2073509276</t>
+          <t>1480000034</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2073509276</v>
+        <v>1480000034</v>
       </c>
       <c r="E3" t="n">
-        <v>2.29</v>
+        <v>4.69</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Turkey Hill Lemonade</t>
+          <t>Mott's 100% Apple Juice</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-06-10T13:40:05.953709</t>
+          <t>2025-06-10T13:40:00.616644</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>18000287949</v>
+        <v>14800002294</v>
       </c>
       <c r="B4" t="n">
-        <v>6.49</v>
+        <v>5.29</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1800028794</t>
+          <t>1480000229</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1800028794</v>
+        <v>1480000229</v>
       </c>
       <c r="E4" t="n">
-        <v>5.29</v>
+        <v>4.99</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Pillsbury Pie Crusts - 2 ct</t>
+          <t>Mott's 100% Apple Juice Original - 6 pk</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-06-10T13:34:48.489528</t>
+          <t>2025-06-10T13:40:03.663830</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>14800002294</v>
+        <v>10900003308</v>
       </c>
       <c r="B5" t="n">
-        <v>5.29</v>
+        <v>3.29</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1480000229</t>
+          <t>1090000330</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1480000229</v>
+        <v>1090000330</v>
       </c>
       <c r="E5" t="n">
-        <v>4.99</v>
+        <v>3.39</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Mott's 100% Apple Juice Original - 6 pk</t>
+          <t>Reynolds Kitchens Cut-Rite Wax Paper 12 Inch Wide</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-06-10T13:40:03.663830</t>
+          <t>2025-06-10T14:23:00.799800</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>13000011105</v>
+        <v>16000275263</v>
       </c>
       <c r="B6" t="n">
-        <v>8.99</v>
+        <v>6.49</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1300001110</t>
+          <t>1600027526</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1300001110</v>
+        <v>1600027526</v>
       </c>
       <c r="E6" t="n">
-        <v>5.99</v>
+        <v>3</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Heinz No Sugar Added Tomato Ketchup</t>
+          <t>Cheerios Gluten Free Cereal</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-06-10T14:00:35.758113</t>
+          <t>2025-06-10T14:13:19.095321</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>13000006057</v>
+        <v>16000125063</v>
       </c>
       <c r="B7" t="n">
-        <v>7.49</v>
+        <v>7.99</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1300000605</t>
+          <t>1600012506</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1300000605</v>
+        <v>1600012506</v>
       </c>
       <c r="E7" t="n">
-        <v>5.29</v>
+        <v>5.79</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Heinz Tomato Ketchup</t>
+          <t>Cheerios Gluten Free Honey Nut Cereal Large Size</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-06-10T14:00:17.004891</t>
+          <t>2025-06-10T14:13:19.083022</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>16000106109</v>
+        <v>13000011105</v>
       </c>
       <c r="B8" t="n">
-        <v>6.99</v>
+        <v>8.99</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1600010610</t>
+          <t>1300001110</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1600010610</v>
+        <v>1300001110</v>
       </c>
       <c r="E8" t="n">
-        <v>6.49</v>
+        <v>5.99</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Gold Medal Bleached All Purpose Flour</t>
+          <t>Heinz No Sugar Added Tomato Ketchup</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-06-10T13:56:12.498804</t>
+          <t>2025-06-10T14:00:35.758113</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>14800000344</v>
+        <v>18000817788</v>
       </c>
       <c r="B9" t="n">
-        <v>4.99</v>
+        <v>6.29</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1480000034</t>
+          <t>1800081778</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1480000034</v>
+        <v>1800081778</v>
       </c>
       <c r="E9" t="n">
-        <v>4.69</v>
+        <v>3.99</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Mott's 100% Apple Juice</t>
+          <t>Pillsbury Chocolate Chip Cookie Dough - 24 ct</t>
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-06-10T13:40:00.616644</t>
+          <t>2025-06-10T13:34:35.324080</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9800895007</v>
+        <v>13000006057</v>
       </c>
       <c r="B10" t="n">
-        <v>5.49</v>
+        <v>7.49</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>980089500</t>
+          <t>1300000605</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>980089500</v>
+        <v>1300000605</v>
       </c>
       <c r="E10" t="n">
         <v>5.29</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Nutella Hazelnut Spread with Cocoa</t>
+          <t>Heinz Tomato Ketchup</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-06-10T14:00:20.363909</t>
+          <t>2025-06-10T14:00:17.004891</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>16000275263</v>
+        <v>10900000185</v>
       </c>
       <c r="B11" t="n">
-        <v>6.49</v>
+        <v>14.99</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1600027526</t>
+          <t>1090000018</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>1600027526</v>
+        <v>1090000018</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>12.79</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Cheerios Gluten Free Cereal</t>
+          <t>Reynolds Wrap Aluminum Foil 12 Inch Wide</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-06-10T14:13:19.095321</t>
+          <t>2025-06-10T14:23:03.431864</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>16000123991</v>
+        <v>16000124790</v>
       </c>
       <c r="B12" t="n">
         <v>6.99</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1600012399</t>
+          <t>1600012479</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1600012399</v>
+        <v>1600012479</v>
       </c>
       <c r="E12" t="n">
         <v>3</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Lucky Charms Gluten Free Cereal with Marshmallows</t>
+          <t>Cheerios Gluten Free Honey Nut Cereal</t>
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-06-10T14:13:19.091556</t>
+          <t>2025-06-10T14:13:19.085881</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>16000125063</v>
+        <v>16000106109</v>
       </c>
       <c r="B13" t="n">
-        <v>7.99</v>
+        <v>6.99</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1600012506</t>
+          <t>1600010610</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>1600012506</v>
+        <v>1600010610</v>
       </c>
       <c r="E13" t="n">
-        <v>5.79</v>
+        <v>6.49</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Cheerios Gluten Free Honey Nut Cereal Large Size</t>
+          <t>Gold Medal Bleached All Purpose Flour</t>
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-06-10T14:13:19.083022</t>
+          <t>2025-06-10T13:56:12.498804</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>16000487949</v>
+        <v>16000107106</v>
       </c>
       <c r="B14" t="n">
-        <v>6.49</v>
+        <v>3.99</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1600048794</t>
+          <t>1600010710</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>1600048794</v>
+        <v>1600010710</v>
       </c>
       <c r="E14" t="n">
-        <v>5.99</v>
+        <v>3.99</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Rice Chex Gluten Free Cereal</t>
+          <t>Gold Medal Bleached All Purpose Flour</t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-06-10T14:13:40.582721</t>
+          <t>2025-06-10T13:56:19.422336</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>16000487727</v>
+        <v>16000123991</v>
       </c>
       <c r="B15" t="n">
-        <v>7.49</v>
+        <v>6.99</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>1600048772</t>
+          <t>1600012399</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>1600048772</v>
+        <v>1600012399</v>
       </c>
       <c r="E15" t="n">
-        <v>5.49</v>
+        <v>3</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Cheerios Gluten Free Cereal Large Size</t>
+          <t>Lucky Charms Gluten Free Cereal with Marshmallows</t>
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-06-10T14:13:19.088798</t>
+          <t>2025-06-10T14:13:19.091556</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>10900003308</v>
+        <v>18000287949</v>
       </c>
       <c r="B16" t="n">
-        <v>3.29</v>
+        <v>6.49</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1090000330</t>
+          <t>1800028794</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>1090000330</v>
+        <v>1800028794</v>
       </c>
       <c r="E16" t="n">
-        <v>3.39</v>
+        <v>5.29</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Reynolds Kitchens Cut-Rite Wax Paper 12 Inch Wide</t>
+          <t>Pillsbury Pie Crusts - 2 ct</t>
         </is>
       </c>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-06-10T14:23:00.799800</t>
+          <t>2025-06-10T13:34:48.489528</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>16000107106</v>
+        <v>10900743310</v>
       </c>
       <c r="B17" t="n">
-        <v>3.99</v>
+        <v>4.99</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1600010710</t>
+          <t>1090074331</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>1600010710</v>
+        <v>1090074331</v>
       </c>
       <c r="E17" t="n">
-        <v>3.99</v>
+        <v>4.69</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Gold Medal Bleached All Purpose Flour</t>
+          <t>Reynolds Kitchens Parchment Paper 15 Inch Wide</t>
         </is>
       </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2025-06-10T13:56:19.422336</t>
+          <t>2025-06-10T14:23:09.106409</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>10900743310</v>
+        <v>16000122543</v>
       </c>
       <c r="B18" t="n">
-        <v>4.99</v>
+        <v>6.99</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1090074331</t>
+          <t>1600012254</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>1090074331</v>
+        <v>1600012254</v>
       </c>
       <c r="E18" t="n">
-        <v>4.69</v>
+        <v>3</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Reynolds Kitchens Parchment Paper 15 Inch Wide</t>
+          <t>Cinnamon Toast Crunch Cereal</t>
         </is>
       </c>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2025-06-10T14:23:09.106409</t>
+          <t>2025-06-10T14:13:19.086829</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>13000007993</v>
+        <v>9800895007</v>
       </c>
       <c r="B19" t="n">
-        <v>4.29</v>
+        <v>5.49</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1300000799</t>
+          <t>980089500</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>1300000799</v>
+        <v>980089500</v>
       </c>
       <c r="E19" t="n">
         <v>5.29</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Heinz No Sugar Added Tomato Ketchup</t>
+          <t>Nutella Hazelnut Spread with Cocoa</t>
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2025-06-10T14:03:05.305959</t>
+          <t>2025-06-10T14:00:20.363909</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>16000122543</v>
+        <v>16000487949</v>
       </c>
       <c r="B20" t="n">
-        <v>6.99</v>
+        <v>6.49</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1600012254</t>
+          <t>1600048794</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>1600012254</v>
+        <v>1600048794</v>
       </c>
       <c r="E20" t="n">
-        <v>3</v>
+        <v>5.99</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Cinnamon Toast Crunch Cereal</t>
+          <t>Rice Chex Gluten Free Cereal</t>
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2025-06-10T14:13:19.086829</t>
+          <t>2025-06-10T14:13:40.582721</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>18000817788</v>
+        <v>13000007993</v>
       </c>
       <c r="B21" t="n">
-        <v>6.29</v>
+        <v>4.29</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1800081778</t>
+          <t>1300000799</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>1800081778</v>
+        <v>1300000799</v>
       </c>
       <c r="E21" t="n">
-        <v>3.99</v>
+        <v>5.29</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Pillsbury Chocolate Chip Cookie Dough - 24 ct</t>
+          <t>Heinz No Sugar Added Tomato Ketchup</t>
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2025-06-10T13:34:35.324080</t>
+          <t>2025-06-10T14:03:05.305959</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>10900000185</v>
+        <v>16000487727</v>
       </c>
       <c r="B22" t="n">
-        <v>14.99</v>
+        <v>7.49</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1090000018</t>
+          <t>1600048772</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>1090000018</v>
+        <v>1600048772</v>
       </c>
       <c r="E22" t="n">
-        <v>12.79</v>
+        <v>5.49</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Reynolds Wrap Aluminum Foil 12 Inch Wide</t>
+          <t>Cheerios Gluten Free Cereal Large Size</t>
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2025-06-10T14:23:03.431864</t>
+          <t>2025-06-10T14:13:19.088798</t>
         </is>
       </c>
     </row>
@@ -1169,631 +1169,631 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>16000124790</v>
+        <v>20735092767</v>
       </c>
       <c r="B2" t="n">
-        <v>6.99</v>
+        <v>2.79</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1600012479</t>
+          <t>2073509276</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1600012479</v>
+        <v>2073509276</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>2.29</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Cheerios Gluten Free Honey Nut Cereal</t>
+          <t>Turkey Hill Lemonade</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-06-10T14:13:19.085881</t>
+          <t>2025-06-10T13:40:05.953709</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>20735092767</v>
+        <v>14800000344</v>
       </c>
       <c r="B3" t="n">
-        <v>2.79</v>
+        <v>4.99</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2073509276</t>
+          <t>1480000034</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2073509276</v>
+        <v>1480000034</v>
       </c>
       <c r="E3" t="n">
-        <v>2.29</v>
+        <v>4.69</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Turkey Hill Lemonade</t>
+          <t>Mott's 100% Apple Juice</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-06-10T13:40:05.953709</t>
+          <t>2025-06-10T13:40:00.616644</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>18000287949</v>
+        <v>14800002294</v>
       </c>
       <c r="B4" t="n">
-        <v>6.49</v>
+        <v>5.29</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1800028794</t>
+          <t>1480000229</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1800028794</v>
+        <v>1480000229</v>
       </c>
       <c r="E4" t="n">
-        <v>5.29</v>
+        <v>4.99</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Pillsbury Pie Crusts - 2 ct</t>
+          <t>Mott's 100% Apple Juice Original - 6 pk</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-06-10T13:34:48.489528</t>
+          <t>2025-06-10T13:40:03.663830</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>14800002294</v>
+        <v>10900003308</v>
       </c>
       <c r="B5" t="n">
-        <v>5.29</v>
+        <v>3.29</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1480000229</t>
+          <t>1090000330</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1480000229</v>
+        <v>1090000330</v>
       </c>
       <c r="E5" t="n">
-        <v>4.99</v>
+        <v>3.39</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Mott's 100% Apple Juice Original - 6 pk</t>
+          <t>Reynolds Kitchens Cut-Rite Wax Paper 12 Inch Wide</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-06-10T13:40:03.663830</t>
+          <t>2025-06-10T14:23:00.799800</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>13000011105</v>
+        <v>16000275263</v>
       </c>
       <c r="B6" t="n">
-        <v>8.99</v>
+        <v>6.49</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1300001110</t>
+          <t>1600027526</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1300001110</v>
+        <v>1600027526</v>
       </c>
       <c r="E6" t="n">
-        <v>5.99</v>
+        <v>3</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Heinz No Sugar Added Tomato Ketchup</t>
+          <t>Cheerios Gluten Free Cereal</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-06-10T14:00:35.758113</t>
+          <t>2025-06-10T14:13:19.095321</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>13000006057</v>
+        <v>16000125063</v>
       </c>
       <c r="B7" t="n">
-        <v>7.49</v>
+        <v>7.99</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1300000605</t>
+          <t>1600012506</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1300000605</v>
+        <v>1600012506</v>
       </c>
       <c r="E7" t="n">
-        <v>5.29</v>
+        <v>5.79</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Heinz Tomato Ketchup</t>
+          <t>Cheerios Gluten Free Honey Nut Cereal Large Size</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-06-10T14:00:17.004891</t>
+          <t>2025-06-10T14:13:19.083022</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>16000106109</v>
+        <v>13000011105</v>
       </c>
       <c r="B8" t="n">
-        <v>6.99</v>
+        <v>8.99</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1600010610</t>
+          <t>1300001110</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1600010610</v>
+        <v>1300001110</v>
       </c>
       <c r="E8" t="n">
-        <v>6.49</v>
+        <v>5.99</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Gold Medal Bleached All Purpose Flour</t>
+          <t>Heinz No Sugar Added Tomato Ketchup</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-06-10T13:56:12.498804</t>
+          <t>2025-06-10T14:00:35.758113</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>14800000344</v>
+        <v>18000817788</v>
       </c>
       <c r="B9" t="n">
-        <v>4.99</v>
+        <v>6.29</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1480000034</t>
+          <t>1800081778</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1480000034</v>
+        <v>1800081778</v>
       </c>
       <c r="E9" t="n">
-        <v>4.69</v>
+        <v>3.99</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Mott's 100% Apple Juice</t>
+          <t>Pillsbury Chocolate Chip Cookie Dough - 24 ct</t>
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-06-10T13:40:00.616644</t>
+          <t>2025-06-10T13:34:35.324080</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9800895007</v>
+        <v>13000006057</v>
       </c>
       <c r="B10" t="n">
-        <v>5.49</v>
+        <v>7.49</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>980089500</t>
+          <t>1300000605</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>980089500</v>
+        <v>1300000605</v>
       </c>
       <c r="E10" t="n">
         <v>5.29</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Nutella Hazelnut Spread with Cocoa</t>
+          <t>Heinz Tomato Ketchup</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-06-10T14:00:20.363909</t>
+          <t>2025-06-10T14:00:17.004891</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>16000275263</v>
+        <v>10900000185</v>
       </c>
       <c r="B11" t="n">
-        <v>6.49</v>
+        <v>14.99</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1600027526</t>
+          <t>1090000018</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>1600027526</v>
+        <v>1090000018</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>12.79</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Cheerios Gluten Free Cereal</t>
+          <t>Reynolds Wrap Aluminum Foil 12 Inch Wide</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-06-10T14:13:19.095321</t>
+          <t>2025-06-10T14:23:03.431864</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>16000123991</v>
+        <v>16000124790</v>
       </c>
       <c r="B12" t="n">
         <v>6.99</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1600012399</t>
+          <t>1600012479</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1600012399</v>
+        <v>1600012479</v>
       </c>
       <c r="E12" t="n">
         <v>3</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Lucky Charms Gluten Free Cereal with Marshmallows</t>
+          <t>Cheerios Gluten Free Honey Nut Cereal</t>
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-06-10T14:13:19.091556</t>
+          <t>2025-06-10T14:13:19.085881</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>16000125063</v>
+        <v>16000106109</v>
       </c>
       <c r="B13" t="n">
-        <v>7.99</v>
+        <v>6.99</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1600012506</t>
+          <t>1600010610</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>1600012506</v>
+        <v>1600010610</v>
       </c>
       <c r="E13" t="n">
-        <v>5.79</v>
+        <v>6.49</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Cheerios Gluten Free Honey Nut Cereal Large Size</t>
+          <t>Gold Medal Bleached All Purpose Flour</t>
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-06-10T14:13:19.083022</t>
+          <t>2025-06-10T13:56:12.498804</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>16000487949</v>
+        <v>16000107106</v>
       </c>
       <c r="B14" t="n">
-        <v>6.49</v>
+        <v>3.99</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1600048794</t>
+          <t>1600010710</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>1600048794</v>
+        <v>1600010710</v>
       </c>
       <c r="E14" t="n">
-        <v>5.99</v>
+        <v>3.99</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Rice Chex Gluten Free Cereal</t>
+          <t>Gold Medal Bleached All Purpose Flour</t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-06-10T14:13:40.582721</t>
+          <t>2025-06-10T13:56:19.422336</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>16000487727</v>
+        <v>16000123991</v>
       </c>
       <c r="B15" t="n">
-        <v>7.49</v>
+        <v>6.99</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>1600048772</t>
+          <t>1600012399</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>1600048772</v>
+        <v>1600012399</v>
       </c>
       <c r="E15" t="n">
-        <v>5.49</v>
+        <v>3</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Cheerios Gluten Free Cereal Large Size</t>
+          <t>Lucky Charms Gluten Free Cereal with Marshmallows</t>
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-06-10T14:13:19.088798</t>
+          <t>2025-06-10T14:13:19.091556</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>10900003308</v>
+        <v>18000287949</v>
       </c>
       <c r="B16" t="n">
-        <v>3.29</v>
+        <v>6.49</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1090000330</t>
+          <t>1800028794</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>1090000330</v>
+        <v>1800028794</v>
       </c>
       <c r="E16" t="n">
-        <v>3.39</v>
+        <v>5.29</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Reynolds Kitchens Cut-Rite Wax Paper 12 Inch Wide</t>
+          <t>Pillsbury Pie Crusts - 2 ct</t>
         </is>
       </c>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-06-10T14:23:00.799800</t>
+          <t>2025-06-10T13:34:48.489528</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>16000107106</v>
+        <v>10900743310</v>
       </c>
       <c r="B17" t="n">
-        <v>3.99</v>
+        <v>4.99</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1600010710</t>
+          <t>1090074331</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>1600010710</v>
+        <v>1090074331</v>
       </c>
       <c r="E17" t="n">
-        <v>3.99</v>
+        <v>4.69</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Gold Medal Bleached All Purpose Flour</t>
+          <t>Reynolds Kitchens Parchment Paper 15 Inch Wide</t>
         </is>
       </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2025-06-10T13:56:19.422336</t>
+          <t>2025-06-10T14:23:09.106409</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>10900743310</v>
+        <v>16000122543</v>
       </c>
       <c r="B18" t="n">
-        <v>4.99</v>
+        <v>6.99</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1090074331</t>
+          <t>1600012254</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>1090074331</v>
+        <v>1600012254</v>
       </c>
       <c r="E18" t="n">
-        <v>4.69</v>
+        <v>3</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Reynolds Kitchens Parchment Paper 15 Inch Wide</t>
+          <t>Cinnamon Toast Crunch Cereal</t>
         </is>
       </c>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2025-06-10T14:23:09.106409</t>
+          <t>2025-06-10T14:13:19.086829</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>13000007993</v>
+        <v>9800895007</v>
       </c>
       <c r="B19" t="n">
-        <v>4.29</v>
+        <v>5.49</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1300000799</t>
+          <t>980089500</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>1300000799</v>
+        <v>980089500</v>
       </c>
       <c r="E19" t="n">
         <v>5.29</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Heinz No Sugar Added Tomato Ketchup</t>
+          <t>Nutella Hazelnut Spread with Cocoa</t>
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2025-06-10T14:03:05.305959</t>
+          <t>2025-06-10T14:00:20.363909</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>16000122543</v>
+        <v>16000487949</v>
       </c>
       <c r="B20" t="n">
-        <v>6.99</v>
+        <v>6.49</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1600012254</t>
+          <t>1600048794</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>1600012254</v>
+        <v>1600048794</v>
       </c>
       <c r="E20" t="n">
-        <v>3</v>
+        <v>5.99</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Cinnamon Toast Crunch Cereal</t>
+          <t>Rice Chex Gluten Free Cereal</t>
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2025-06-10T14:13:19.086829</t>
+          <t>2025-06-10T14:13:40.582721</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>18000817788</v>
+        <v>13000007993</v>
       </c>
       <c r="B21" t="n">
-        <v>6.29</v>
+        <v>4.29</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1800081778</t>
+          <t>1300000799</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>1800081778</v>
+        <v>1300000799</v>
       </c>
       <c r="E21" t="n">
-        <v>3.99</v>
+        <v>5.29</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Pillsbury Chocolate Chip Cookie Dough - 24 ct</t>
+          <t>Heinz No Sugar Added Tomato Ketchup</t>
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2025-06-10T13:34:35.324080</t>
+          <t>2025-06-10T14:03:05.305959</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>10900000185</v>
+        <v>16000487727</v>
       </c>
       <c r="B22" t="n">
-        <v>14.99</v>
+        <v>7.49</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1090000018</t>
+          <t>1600048772</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>1090000018</v>
+        <v>1600048772</v>
       </c>
       <c r="E22" t="n">
-        <v>12.79</v>
+        <v>5.49</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Reynolds Wrap Aluminum Foil 12 Inch Wide</t>
+          <t>Cheerios Gluten Free Cereal Large Size</t>
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2025-06-10T14:23:03.431864</t>
+          <t>2025-06-10T14:13:19.088798</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added drag and drop functionality + fixed dimming layer to be dynamic
</commit_message>
<xml_diff>
--- a/scraplingAdaptationHana/giant/giant_price_compare/giant_foods_comparison.xlsx
+++ b/scraplingAdaptationHana/giant/giant_price_compare/giant_foods_comparison.xlsx
@@ -478,631 +478,631 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>20735092767</v>
+        <v>10900003308</v>
       </c>
       <c r="B2" t="n">
-        <v>2.79</v>
+        <v>3.29</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2073509276</t>
+          <t>1090000330</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2073509276</v>
+        <v>1090000330</v>
       </c>
       <c r="E2" t="n">
-        <v>2.29</v>
+        <v>3.39</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Turkey Hill Lemonade</t>
+          <t>Reynolds Kitchens Cut-Rite Wax Paper 12 Inch Wide</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-06-10T13:40:05.953709</t>
+          <t>2025-06-10T14:23:00.799800</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>14800000344</v>
+        <v>18000817788</v>
       </c>
       <c r="B3" t="n">
-        <v>4.99</v>
+        <v>6.29</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1480000034</t>
+          <t>1800081778</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1480000034</v>
+        <v>1800081778</v>
       </c>
       <c r="E3" t="n">
-        <v>4.69</v>
+        <v>3.99</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Mott's 100% Apple Juice</t>
+          <t>Pillsbury Chocolate Chip Cookie Dough - 24 ct</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-06-10T13:40:00.616644</t>
+          <t>2025-06-10T13:34:35.324080</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>14800002294</v>
+        <v>16000123991</v>
       </c>
       <c r="B4" t="n">
-        <v>5.29</v>
+        <v>6.99</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1480000229</t>
+          <t>1600012399</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1480000229</v>
+        <v>1600012399</v>
       </c>
       <c r="E4" t="n">
-        <v>4.99</v>
+        <v>3</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Mott's 100% Apple Juice Original - 6 pk</t>
+          <t>Lucky Charms Gluten Free Cereal with Marshmallows</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-06-10T13:40:03.663830</t>
+          <t>2025-06-10T14:13:19.091556</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>10900003308</v>
+        <v>16000125063</v>
       </c>
       <c r="B5" t="n">
-        <v>3.29</v>
+        <v>7.99</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1090000330</t>
+          <t>1600012506</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1090000330</v>
+        <v>1600012506</v>
       </c>
       <c r="E5" t="n">
-        <v>3.39</v>
+        <v>5.79</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Reynolds Kitchens Cut-Rite Wax Paper 12 Inch Wide</t>
+          <t>Cheerios Gluten Free Honey Nut Cereal Large Size</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-06-10T14:23:00.799800</t>
+          <t>2025-06-10T14:13:19.083022</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>16000275263</v>
+        <v>16000487949</v>
       </c>
       <c r="B6" t="n">
         <v>6.49</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1600027526</t>
+          <t>1600048794</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1600027526</v>
+        <v>1600048794</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>5.99</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Cheerios Gluten Free Cereal</t>
+          <t>Rice Chex Gluten Free Cereal</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-06-10T14:13:19.095321</t>
+          <t>2025-06-10T14:13:40.582721</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>16000125063</v>
+        <v>16000124790</v>
       </c>
       <c r="B7" t="n">
-        <v>7.99</v>
+        <v>6.99</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1600012506</t>
+          <t>1600012479</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1600012506</v>
+        <v>1600012479</v>
       </c>
       <c r="E7" t="n">
-        <v>5.79</v>
+        <v>3</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Cheerios Gluten Free Honey Nut Cereal Large Size</t>
+          <t>Cheerios Gluten Free Honey Nut Cereal</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-06-10T14:13:19.083022</t>
+          <t>2025-06-10T14:13:19.085881</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>13000011105</v>
+        <v>16000122543</v>
       </c>
       <c r="B8" t="n">
-        <v>8.99</v>
+        <v>6.99</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1300001110</t>
+          <t>1600012254</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1300001110</v>
+        <v>1600012254</v>
       </c>
       <c r="E8" t="n">
-        <v>5.99</v>
+        <v>3</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Heinz No Sugar Added Tomato Ketchup</t>
+          <t>Cinnamon Toast Crunch Cereal</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-06-10T14:00:35.758113</t>
+          <t>2025-06-10T14:13:19.086829</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>18000817788</v>
+        <v>13000011105</v>
       </c>
       <c r="B9" t="n">
-        <v>6.29</v>
+        <v>8.99</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1800081778</t>
+          <t>1300001110</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1800081778</v>
+        <v>1300001110</v>
       </c>
       <c r="E9" t="n">
-        <v>3.99</v>
+        <v>5.99</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Pillsbury Chocolate Chip Cookie Dough - 24 ct</t>
+          <t>Heinz No Sugar Added Tomato Ketchup</t>
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-06-10T13:34:35.324080</t>
+          <t>2025-06-10T14:00:35.758113</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>13000006057</v>
+        <v>16000106109</v>
       </c>
       <c r="B10" t="n">
-        <v>7.49</v>
+        <v>6.99</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1300000605</t>
+          <t>1600010610</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1300000605</v>
+        <v>1600010610</v>
       </c>
       <c r="E10" t="n">
-        <v>5.29</v>
+        <v>6.49</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Heinz Tomato Ketchup</t>
+          <t>Gold Medal Bleached All Purpose Flour</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-06-10T14:00:17.004891</t>
+          <t>2025-06-10T13:56:12.498804</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10900000185</v>
+        <v>10900743310</v>
       </c>
       <c r="B11" t="n">
-        <v>14.99</v>
+        <v>4.99</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1090000018</t>
+          <t>1090074331</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>1090000018</v>
+        <v>1090074331</v>
       </c>
       <c r="E11" t="n">
-        <v>12.79</v>
+        <v>4.69</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Reynolds Wrap Aluminum Foil 12 Inch Wide</t>
+          <t>Reynolds Kitchens Parchment Paper 15 Inch Wide</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-06-10T14:23:03.431864</t>
+          <t>2025-06-10T14:23:09.106409</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>16000124790</v>
+        <v>20735092767</v>
       </c>
       <c r="B12" t="n">
-        <v>6.99</v>
+        <v>2.79</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1600012479</t>
+          <t>2073509276</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1600012479</v>
+        <v>2073509276</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>2.29</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Cheerios Gluten Free Honey Nut Cereal</t>
+          <t>Turkey Hill Lemonade</t>
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-06-10T14:13:19.085881</t>
+          <t>2025-06-10T13:40:05.953709</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>16000106109</v>
+        <v>13000007993</v>
       </c>
       <c r="B13" t="n">
-        <v>6.99</v>
+        <v>4.29</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1600010610</t>
+          <t>1300000799</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>1600010610</v>
+        <v>1300000799</v>
       </c>
       <c r="E13" t="n">
-        <v>6.49</v>
+        <v>5.29</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Gold Medal Bleached All Purpose Flour</t>
+          <t>Heinz No Sugar Added Tomato Ketchup</t>
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-06-10T13:56:12.498804</t>
+          <t>2025-06-10T14:03:05.305959</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>16000107106</v>
+        <v>14800000344</v>
       </c>
       <c r="B14" t="n">
-        <v>3.99</v>
+        <v>4.99</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1600010710</t>
+          <t>1480000034</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>1600010710</v>
+        <v>1480000034</v>
       </c>
       <c r="E14" t="n">
-        <v>3.99</v>
+        <v>4.69</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Gold Medal Bleached All Purpose Flour</t>
+          <t>Mott's 100% Apple Juice</t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-06-10T13:56:19.422336</t>
+          <t>2025-06-10T13:40:00.616644</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>16000123991</v>
+        <v>16000275263</v>
       </c>
       <c r="B15" t="n">
-        <v>6.99</v>
+        <v>6.49</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>1600012399</t>
+          <t>1600027526</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>1600012399</v>
+        <v>1600027526</v>
       </c>
       <c r="E15" t="n">
         <v>3</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Lucky Charms Gluten Free Cereal with Marshmallows</t>
+          <t>Cheerios Gluten Free Cereal</t>
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-06-10T14:13:19.091556</t>
+          <t>2025-06-10T14:13:19.095321</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>18000287949</v>
+        <v>14800002294</v>
       </c>
       <c r="B16" t="n">
-        <v>6.49</v>
+        <v>5.29</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1800028794</t>
+          <t>1480000229</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>1800028794</v>
+        <v>1480000229</v>
       </c>
       <c r="E16" t="n">
-        <v>5.29</v>
+        <v>4.99</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Pillsbury Pie Crusts - 2 ct</t>
+          <t>Mott's 100% Apple Juice Original - 6 pk</t>
         </is>
       </c>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-06-10T13:34:48.489528</t>
+          <t>2025-06-10T13:40:03.663830</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>10900743310</v>
+        <v>9800895007</v>
       </c>
       <c r="B17" t="n">
-        <v>4.99</v>
+        <v>5.49</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1090074331</t>
+          <t>980089500</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>1090074331</v>
+        <v>980089500</v>
       </c>
       <c r="E17" t="n">
-        <v>4.69</v>
+        <v>5.29</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Reynolds Kitchens Parchment Paper 15 Inch Wide</t>
+          <t>Nutella Hazelnut Spread with Cocoa</t>
         </is>
       </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2025-06-10T14:23:09.106409</t>
+          <t>2025-06-10T14:00:20.363909</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>16000122543</v>
+        <v>18000287949</v>
       </c>
       <c r="B18" t="n">
-        <v>6.99</v>
+        <v>6.49</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1600012254</t>
+          <t>1800028794</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>1600012254</v>
+        <v>1800028794</v>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>5.29</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Cinnamon Toast Crunch Cereal</t>
+          <t>Pillsbury Pie Crusts - 2 ct</t>
         </is>
       </c>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2025-06-10T14:13:19.086829</t>
+          <t>2025-06-10T13:34:48.489528</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>9800895007</v>
+        <v>16000487727</v>
       </c>
       <c r="B19" t="n">
+        <v>7.49</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>1600048772</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>1600048772</v>
+      </c>
+      <c r="E19" t="n">
         <v>5.49</v>
       </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>980089500</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>980089500</v>
-      </c>
-      <c r="E19" t="n">
-        <v>5.29</v>
-      </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Nutella Hazelnut Spread with Cocoa</t>
+          <t>Cheerios Gluten Free Cereal Large Size</t>
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2025-06-10T14:00:20.363909</t>
+          <t>2025-06-10T14:13:19.088798</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>16000487949</v>
+        <v>16000107106</v>
       </c>
       <c r="B20" t="n">
-        <v>6.49</v>
+        <v>3.99</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1600048794</t>
+          <t>1600010710</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>1600048794</v>
+        <v>1600010710</v>
       </c>
       <c r="E20" t="n">
-        <v>5.99</v>
+        <v>3.99</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Rice Chex Gluten Free Cereal</t>
+          <t>Gold Medal Bleached All Purpose Flour</t>
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2025-06-10T14:13:40.582721</t>
+          <t>2025-06-10T13:56:19.422336</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>13000007993</v>
+        <v>13000006057</v>
       </c>
       <c r="B21" t="n">
-        <v>4.29</v>
+        <v>7.49</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1300000799</t>
+          <t>1300000605</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>1300000799</v>
+        <v>1300000605</v>
       </c>
       <c r="E21" t="n">
         <v>5.29</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Heinz No Sugar Added Tomato Ketchup</t>
+          <t>Heinz Tomato Ketchup</t>
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2025-06-10T14:03:05.305959</t>
+          <t>2025-06-10T14:00:17.004891</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>16000487727</v>
+        <v>10900000185</v>
       </c>
       <c r="B22" t="n">
-        <v>7.49</v>
+        <v>14.99</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1600048772</t>
+          <t>1090000018</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>1600048772</v>
+        <v>1090000018</v>
       </c>
       <c r="E22" t="n">
-        <v>5.49</v>
+        <v>12.79</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Cheerios Gluten Free Cereal Large Size</t>
+          <t>Reynolds Wrap Aluminum Foil 12 Inch Wide</t>
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2025-06-10T14:13:19.088798</t>
+          <t>2025-06-10T14:23:03.431864</t>
         </is>
       </c>
     </row>
@@ -1169,631 +1169,631 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>20735092767</v>
+        <v>10900003308</v>
       </c>
       <c r="B2" t="n">
-        <v>2.79</v>
+        <v>3.29</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2073509276</t>
+          <t>1090000330</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2073509276</v>
+        <v>1090000330</v>
       </c>
       <c r="E2" t="n">
-        <v>2.29</v>
+        <v>3.39</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Turkey Hill Lemonade</t>
+          <t>Reynolds Kitchens Cut-Rite Wax Paper 12 Inch Wide</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-06-10T13:40:05.953709</t>
+          <t>2025-06-10T14:23:00.799800</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>14800000344</v>
+        <v>18000817788</v>
       </c>
       <c r="B3" t="n">
-        <v>4.99</v>
+        <v>6.29</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1480000034</t>
+          <t>1800081778</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1480000034</v>
+        <v>1800081778</v>
       </c>
       <c r="E3" t="n">
-        <v>4.69</v>
+        <v>3.99</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Mott's 100% Apple Juice</t>
+          <t>Pillsbury Chocolate Chip Cookie Dough - 24 ct</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-06-10T13:40:00.616644</t>
+          <t>2025-06-10T13:34:35.324080</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>14800002294</v>
+        <v>16000123991</v>
       </c>
       <c r="B4" t="n">
-        <v>5.29</v>
+        <v>6.99</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1480000229</t>
+          <t>1600012399</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1480000229</v>
+        <v>1600012399</v>
       </c>
       <c r="E4" t="n">
-        <v>4.99</v>
+        <v>3</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Mott's 100% Apple Juice Original - 6 pk</t>
+          <t>Lucky Charms Gluten Free Cereal with Marshmallows</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-06-10T13:40:03.663830</t>
+          <t>2025-06-10T14:13:19.091556</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>10900003308</v>
+        <v>16000125063</v>
       </c>
       <c r="B5" t="n">
-        <v>3.29</v>
+        <v>7.99</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1090000330</t>
+          <t>1600012506</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1090000330</v>
+        <v>1600012506</v>
       </c>
       <c r="E5" t="n">
-        <v>3.39</v>
+        <v>5.79</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Reynolds Kitchens Cut-Rite Wax Paper 12 Inch Wide</t>
+          <t>Cheerios Gluten Free Honey Nut Cereal Large Size</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-06-10T14:23:00.799800</t>
+          <t>2025-06-10T14:13:19.083022</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>16000275263</v>
+        <v>16000487949</v>
       </c>
       <c r="B6" t="n">
         <v>6.49</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1600027526</t>
+          <t>1600048794</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1600027526</v>
+        <v>1600048794</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>5.99</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Cheerios Gluten Free Cereal</t>
+          <t>Rice Chex Gluten Free Cereal</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-06-10T14:13:19.095321</t>
+          <t>2025-06-10T14:13:40.582721</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>16000125063</v>
+        <v>16000124790</v>
       </c>
       <c r="B7" t="n">
-        <v>7.99</v>
+        <v>6.99</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1600012506</t>
+          <t>1600012479</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1600012506</v>
+        <v>1600012479</v>
       </c>
       <c r="E7" t="n">
-        <v>5.79</v>
+        <v>3</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Cheerios Gluten Free Honey Nut Cereal Large Size</t>
+          <t>Cheerios Gluten Free Honey Nut Cereal</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-06-10T14:13:19.083022</t>
+          <t>2025-06-10T14:13:19.085881</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>13000011105</v>
+        <v>16000122543</v>
       </c>
       <c r="B8" t="n">
-        <v>8.99</v>
+        <v>6.99</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1300001110</t>
+          <t>1600012254</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1300001110</v>
+        <v>1600012254</v>
       </c>
       <c r="E8" t="n">
-        <v>5.99</v>
+        <v>3</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Heinz No Sugar Added Tomato Ketchup</t>
+          <t>Cinnamon Toast Crunch Cereal</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-06-10T14:00:35.758113</t>
+          <t>2025-06-10T14:13:19.086829</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>18000817788</v>
+        <v>13000011105</v>
       </c>
       <c r="B9" t="n">
-        <v>6.29</v>
+        <v>8.99</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1800081778</t>
+          <t>1300001110</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1800081778</v>
+        <v>1300001110</v>
       </c>
       <c r="E9" t="n">
-        <v>3.99</v>
+        <v>5.99</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Pillsbury Chocolate Chip Cookie Dough - 24 ct</t>
+          <t>Heinz No Sugar Added Tomato Ketchup</t>
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-06-10T13:34:35.324080</t>
+          <t>2025-06-10T14:00:35.758113</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>13000006057</v>
+        <v>16000106109</v>
       </c>
       <c r="B10" t="n">
-        <v>7.49</v>
+        <v>6.99</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1300000605</t>
+          <t>1600010610</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1300000605</v>
+        <v>1600010610</v>
       </c>
       <c r="E10" t="n">
-        <v>5.29</v>
+        <v>6.49</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Heinz Tomato Ketchup</t>
+          <t>Gold Medal Bleached All Purpose Flour</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-06-10T14:00:17.004891</t>
+          <t>2025-06-10T13:56:12.498804</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10900000185</v>
+        <v>10900743310</v>
       </c>
       <c r="B11" t="n">
-        <v>14.99</v>
+        <v>4.99</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1090000018</t>
+          <t>1090074331</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>1090000018</v>
+        <v>1090074331</v>
       </c>
       <c r="E11" t="n">
-        <v>12.79</v>
+        <v>4.69</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Reynolds Wrap Aluminum Foil 12 Inch Wide</t>
+          <t>Reynolds Kitchens Parchment Paper 15 Inch Wide</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-06-10T14:23:03.431864</t>
+          <t>2025-06-10T14:23:09.106409</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>16000124790</v>
+        <v>20735092767</v>
       </c>
       <c r="B12" t="n">
-        <v>6.99</v>
+        <v>2.79</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1600012479</t>
+          <t>2073509276</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1600012479</v>
+        <v>2073509276</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>2.29</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Cheerios Gluten Free Honey Nut Cereal</t>
+          <t>Turkey Hill Lemonade</t>
         </is>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-06-10T14:13:19.085881</t>
+          <t>2025-06-10T13:40:05.953709</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>16000106109</v>
+        <v>13000007993</v>
       </c>
       <c r="B13" t="n">
-        <v>6.99</v>
+        <v>4.29</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1600010610</t>
+          <t>1300000799</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>1600010610</v>
+        <v>1300000799</v>
       </c>
       <c r="E13" t="n">
-        <v>6.49</v>
+        <v>5.29</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Gold Medal Bleached All Purpose Flour</t>
+          <t>Heinz No Sugar Added Tomato Ketchup</t>
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-06-10T13:56:12.498804</t>
+          <t>2025-06-10T14:03:05.305959</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>16000107106</v>
+        <v>14800000344</v>
       </c>
       <c r="B14" t="n">
-        <v>3.99</v>
+        <v>4.99</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1600010710</t>
+          <t>1480000034</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>1600010710</v>
+        <v>1480000034</v>
       </c>
       <c r="E14" t="n">
-        <v>3.99</v>
+        <v>4.69</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Gold Medal Bleached All Purpose Flour</t>
+          <t>Mott's 100% Apple Juice</t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-06-10T13:56:19.422336</t>
+          <t>2025-06-10T13:40:00.616644</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>16000123991</v>
+        <v>16000275263</v>
       </c>
       <c r="B15" t="n">
-        <v>6.99</v>
+        <v>6.49</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>1600012399</t>
+          <t>1600027526</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>1600012399</v>
+        <v>1600027526</v>
       </c>
       <c r="E15" t="n">
         <v>3</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Lucky Charms Gluten Free Cereal with Marshmallows</t>
+          <t>Cheerios Gluten Free Cereal</t>
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-06-10T14:13:19.091556</t>
+          <t>2025-06-10T14:13:19.095321</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>18000287949</v>
+        <v>14800002294</v>
       </c>
       <c r="B16" t="n">
-        <v>6.49</v>
+        <v>5.29</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1800028794</t>
+          <t>1480000229</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>1800028794</v>
+        <v>1480000229</v>
       </c>
       <c r="E16" t="n">
-        <v>5.29</v>
+        <v>4.99</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Pillsbury Pie Crusts - 2 ct</t>
+          <t>Mott's 100% Apple Juice Original - 6 pk</t>
         </is>
       </c>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-06-10T13:34:48.489528</t>
+          <t>2025-06-10T13:40:03.663830</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>10900743310</v>
+        <v>9800895007</v>
       </c>
       <c r="B17" t="n">
-        <v>4.99</v>
+        <v>5.49</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1090074331</t>
+          <t>980089500</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>1090074331</v>
+        <v>980089500</v>
       </c>
       <c r="E17" t="n">
-        <v>4.69</v>
+        <v>5.29</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Reynolds Kitchens Parchment Paper 15 Inch Wide</t>
+          <t>Nutella Hazelnut Spread with Cocoa</t>
         </is>
       </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2025-06-10T14:23:09.106409</t>
+          <t>2025-06-10T14:00:20.363909</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>16000122543</v>
+        <v>18000287949</v>
       </c>
       <c r="B18" t="n">
-        <v>6.99</v>
+        <v>6.49</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1600012254</t>
+          <t>1800028794</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>1600012254</v>
+        <v>1800028794</v>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>5.29</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Cinnamon Toast Crunch Cereal</t>
+          <t>Pillsbury Pie Crusts - 2 ct</t>
         </is>
       </c>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2025-06-10T14:13:19.086829</t>
+          <t>2025-06-10T13:34:48.489528</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>9800895007</v>
+        <v>16000487727</v>
       </c>
       <c r="B19" t="n">
+        <v>7.49</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>1600048772</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>1600048772</v>
+      </c>
+      <c r="E19" t="n">
         <v>5.49</v>
       </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>980089500</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>980089500</v>
-      </c>
-      <c r="E19" t="n">
-        <v>5.29</v>
-      </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Nutella Hazelnut Spread with Cocoa</t>
+          <t>Cheerios Gluten Free Cereal Large Size</t>
         </is>
       </c>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2025-06-10T14:00:20.363909</t>
+          <t>2025-06-10T14:13:19.088798</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>16000487949</v>
+        <v>16000107106</v>
       </c>
       <c r="B20" t="n">
-        <v>6.49</v>
+        <v>3.99</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1600048794</t>
+          <t>1600010710</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>1600048794</v>
+        <v>1600010710</v>
       </c>
       <c r="E20" t="n">
-        <v>5.99</v>
+        <v>3.99</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Rice Chex Gluten Free Cereal</t>
+          <t>Gold Medal Bleached All Purpose Flour</t>
         </is>
       </c>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2025-06-10T14:13:40.582721</t>
+          <t>2025-06-10T13:56:19.422336</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>13000007993</v>
+        <v>13000006057</v>
       </c>
       <c r="B21" t="n">
-        <v>4.29</v>
+        <v>7.49</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1300000799</t>
+          <t>1300000605</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>1300000799</v>
+        <v>1300000605</v>
       </c>
       <c r="E21" t="n">
         <v>5.29</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Heinz No Sugar Added Tomato Ketchup</t>
+          <t>Heinz Tomato Ketchup</t>
         </is>
       </c>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2025-06-10T14:03:05.305959</t>
+          <t>2025-06-10T14:00:17.004891</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>16000487727</v>
+        <v>10900000185</v>
       </c>
       <c r="B22" t="n">
-        <v>7.49</v>
+        <v>14.99</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1600048772</t>
+          <t>1090000018</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>1600048772</v>
+        <v>1090000018</v>
       </c>
       <c r="E22" t="n">
-        <v>5.49</v>
+        <v>12.79</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Cheerios Gluten Free Cereal Large Size</t>
+          <t>Reynolds Wrap Aluminum Foil 12 Inch Wide</t>
         </is>
       </c>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2025-06-10T14:13:19.088798</t>
+          <t>2025-06-10T14:23:03.431864</t>
         </is>
       </c>
     </row>

</xml_diff>